<commit_message>
tried t fix history generators
</commit_message>
<xml_diff>
--- a/SchluterLog.xlsx
+++ b/SchluterLog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Samsung_T5/APP/MXX-git2-/SchulterReproduction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendanoconnor/Desktop/APP/mxx-git2-/SchulterReproduction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7824C38-CBB9-5340-AD2C-C0F9179043E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B6F6BD-2C89-F843-96C9-9EA692B66FCE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{0E031976-A5C9-AA40-B978-4DA5AD1A59FA}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="128">
   <si>
     <t>n_Conv2DLayers</t>
   </si>
@@ -412,6 +412,9 @@
   </si>
   <si>
     <t>withAugsFromWavLocalBlockNorm3StridePoint71FiltNadineValMethod</t>
+  </si>
+  <si>
+    <t>withAugsFromWavLocalBlockNorm3Stride2FiltNadineValMethod</t>
   </si>
 </sst>
 </file>
@@ -970,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C52FB76-D6A8-4443-9969-C23B8B0F28D6}">
   <dimension ref="A1:AO36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3954,17 +3957,17 @@
       <c r="C30" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E30" s="19">
-        <v>0.19819999999999999</v>
-      </c>
-      <c r="F30" s="29">
-        <v>0.93359999999999999</v>
-      </c>
-      <c r="G30" s="25">
-        <v>0.34350000000000003</v>
-      </c>
-      <c r="H30" s="5">
-        <v>0.86529999999999996</v>
+      <c r="E30" s="16">
+        <v>0.22120000000000001</v>
+      </c>
+      <c r="F30" s="16">
+        <v>0.91269999999999996</v>
+      </c>
+      <c r="G30" s="16">
+        <v>0.3372</v>
+      </c>
+      <c r="H30" s="16">
+        <v>0.87590000000000001</v>
       </c>
       <c r="I30" s="7" t="s">
         <v>67</v>
@@ -4040,6 +4043,9 @@
       </c>
       <c r="AG30" s="27">
         <v>1408225</v>
+      </c>
+      <c r="AH30">
+        <v>6</v>
       </c>
       <c r="AI30" s="1">
         <v>1250</v>
@@ -4162,6 +4168,18 @@
       <c r="C32" s="7" t="s">
         <v>126</v>
       </c>
+      <c r="E32" s="16">
+        <v>0.27479999999999999</v>
+      </c>
+      <c r="F32" s="16">
+        <v>0.88680000000000003</v>
+      </c>
+      <c r="G32" s="16">
+        <v>0.36840000000000001</v>
+      </c>
+      <c r="H32" s="16">
+        <v>0.84389999999999998</v>
+      </c>
       <c r="I32" s="7" t="s">
         <v>67</v>
       </c>
@@ -4223,7 +4241,16 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="17:36" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A33" s="28">
+        <v>43675</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>127</v>
+      </c>
       <c r="Q33" s="4">
         <v>625</v>
       </c>
@@ -4282,7 +4309,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="17:36" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.2">
       <c r="Q34" s="4">
         <v>625</v>
       </c>
@@ -4341,7 +4368,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="17:36" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.2">
       <c r="Q35" s="1">
         <v>625</v>
       </c>
@@ -4400,7 +4427,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="17:36" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.2">
       <c r="Q36" s="1">
         <v>625</v>
       </c>

</xml_diff>